<commit_message>
menys ifs a la GUI
</commit_message>
<xml_diff>
--- a/TRIAL_VMIX.xlsx
+++ b/TRIAL_VMIX.xlsx
@@ -1434,7 +1434,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SECTION 5</t>
+          <t>SECTION 2</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -1745,74 +1745,74 @@
       </c>
       <c r="CO2" t="inlineStr">
         <is>
+          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
+        </is>
+      </c>
+      <c r="CP2" t="inlineStr">
+        <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
         </is>
       </c>
-      <c r="CP2" t="inlineStr">
+      <c r="CQ2" t="inlineStr">
+        <is>
+          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
+        </is>
+      </c>
+      <c r="CR2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="CQ2" t="inlineStr">
-        <is>
-          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
-        </is>
-      </c>
-      <c r="CR2" t="inlineStr">
+      <c r="CS2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="CS2" t="inlineStr">
+      <c r="CT2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="CT2" t="inlineStr">
-        <is>
-          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
-        </is>
-      </c>
       <c r="CU2" t="inlineStr">
         <is>
+          <t>ESP</t>
+        </is>
+      </c>
+      <c r="CV2" t="inlineStr">
+        <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="CV2" t="inlineStr">
+      <c r="CW2" t="inlineStr">
+        <is>
+          <t>FRA</t>
+        </is>
+      </c>
+      <c r="CX2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="CW2" t="inlineStr">
-        <is>
-          <t>FRA</t>
-        </is>
-      </c>
-      <c r="CX2" t="inlineStr">
+      <c r="CY2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="CY2" t="inlineStr">
+      <c r="CZ2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="CZ2" t="inlineStr">
-        <is>
-          <t>ESP</t>
-        </is>
-      </c>
       <c r="DA2" t="inlineStr">
         <is>
+          <t>ALEJANDRO MO</t>
+        </is>
+      </c>
+      <c r="DB2" t="inlineStr">
+        <is>
           <t>VINCENT H</t>
         </is>
       </c>
-      <c r="DB2" t="inlineStr">
-        <is>
-          <t>ALEJANDRO MO</t>
-        </is>
-      </c>
       <c r="DC2" t="inlineStr">
         <is>
           <t>NICOLAS V</t>
@@ -1834,10 +1834,10 @@
         </is>
       </c>
       <c r="DG2" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="DH2" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="DI2" t="n">
         <v>0</v>
@@ -1852,10 +1852,10 @@
         <v>0</v>
       </c>
       <c r="DM2" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="DN2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="DO2" t="n">
         <v>0</v>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="DT2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="DU2" t="n">
         <v>0</v>
@@ -1891,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="DZ2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="EA2" t="n">
         <v>0</v>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="EL2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="EM2" t="n">
         <v>0</v>
@@ -1943,14 +1943,14 @@
       </c>
       <c r="EQ2" t="inlineStr">
         <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="ER2" t="inlineStr">
+        <is>
           <t>HER</t>
         </is>
       </c>
-      <c r="ER2" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
       <c r="ES2" t="inlineStr">
         <is>
           <t>VAL</t>
@@ -2005,10 +2005,12 @@
         </is>
       </c>
       <c r="FD2" t="n">
-        <v>10</v>
-      </c>
-      <c r="FE2" t="n">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="FE2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="FF2" t="inlineStr">
         <is>
@@ -2040,32 +2042,32 @@
       </c>
       <c r="FL2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FM2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FN2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FO2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FP2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FQ2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FR2" t="n">
@@ -2073,32 +2075,32 @@
       </c>
       <c r="FS2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FT2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FU2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FV2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FW2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FX2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="FY2" t="n">
@@ -2106,32 +2108,32 @@
       </c>
       <c r="FZ2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GA2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GB2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GC2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GD2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GE2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GF2" t="n">
@@ -2139,32 +2141,32 @@
       </c>
       <c r="GG2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GH2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GI2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GJ2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GK2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GL2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> -</t>
         </is>
       </c>
       <c r="GM2" t="inlineStr">

</xml_diff>

<commit_message>
streamdeck -- controlant secció i player
</commit_message>
<xml_diff>
--- a/TRIAL_VMIX.xlsx
+++ b/TRIAL_VMIX.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FM2"/>
+  <dimension ref="A1:FG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1247,36 +1247,6 @@
           <t>hashtag</t>
         </is>
       </c>
-      <c r="FH1" s="1" t="inlineStr">
-        <is>
-          <t>1_PUNTS_SECCIO</t>
-        </is>
-      </c>
-      <c r="FI1" s="1" t="inlineStr">
-        <is>
-          <t>2_PUNTS_SECCIO</t>
-        </is>
-      </c>
-      <c r="FJ1" s="1" t="inlineStr">
-        <is>
-          <t>3_PUNTS_SECCIO</t>
-        </is>
-      </c>
-      <c r="FK1" s="1" t="inlineStr">
-        <is>
-          <t>4_PUNTS_SECCIO</t>
-        </is>
-      </c>
-      <c r="FL1" s="1" t="inlineStr">
-        <is>
-          <t>5_PUNTS_SECCIO</t>
-        </is>
-      </c>
-      <c r="FM1" s="1" t="inlineStr">
-        <is>
-          <t>6_PUNTS_SECCIO</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1304,7 +1274,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SECTION 1</t>
+          <t>SECTION 5</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -1373,39 +1343,39 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
+          <t>FRA</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>FRA</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>ESP</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>ESP</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
         <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>ESP</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>ESP</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>ESP</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>FRA</t>
-        </is>
-      </c>
       <c r="AD2" t="inlineStr">
         <is>
           <t>GER</t>
@@ -1413,7 +1383,7 @@
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>ALEJANDRO MO</t>
+          <t>VINCENT H</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
@@ -1615,19 +1585,19 @@
       </c>
       <c r="CO2" t="inlineStr">
         <is>
+          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
+        </is>
+      </c>
+      <c r="CP2" t="inlineStr">
+        <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="CP2" t="inlineStr">
+      <c r="CQ2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
         </is>
       </c>
-      <c r="CQ2" t="inlineStr">
-        <is>
-          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
-        </is>
-      </c>
       <c r="CR2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
@@ -1645,19 +1615,19 @@
       </c>
       <c r="CU2" t="inlineStr">
         <is>
+          <t>FRA</t>
+        </is>
+      </c>
+      <c r="CV2" t="inlineStr">
+        <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="CV2" t="inlineStr">
+      <c r="CW2" t="inlineStr">
         <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="CW2" t="inlineStr">
-        <is>
-          <t>FRA</t>
-        </is>
-      </c>
       <c r="CX2" t="inlineStr">
         <is>
           <t>ESP</t>
@@ -1675,14 +1645,14 @@
       </c>
       <c r="DA2" t="inlineStr">
         <is>
+          <t>VINCENT H</t>
+        </is>
+      </c>
+      <c r="DB2" t="inlineStr">
+        <is>
           <t>ALEJANDRO MO</t>
         </is>
       </c>
-      <c r="DB2" t="inlineStr">
-        <is>
-          <t>VINCENT H</t>
-        </is>
-      </c>
       <c r="DC2" t="inlineStr">
         <is>
           <t>NICOLAS V</t>
@@ -1704,10 +1674,10 @@
         </is>
       </c>
       <c r="DG2" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="DH2" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="DI2" t="n">
         <v>0</v>
@@ -1722,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="DM2" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="DN2" t="n">
         <v>0</v>
@@ -1743,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="DT2" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="DU2" t="n">
         <v>0</v>
@@ -1761,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="DZ2" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="EA2" t="n">
         <v>0</v>
@@ -1813,14 +1783,14 @@
       </c>
       <c r="EQ2" t="inlineStr">
         <is>
+          <t>HER</t>
+        </is>
+      </c>
+      <c r="ER2" t="inlineStr">
+        <is>
           <t>MON</t>
         </is>
       </c>
-      <c r="ER2" t="inlineStr">
-        <is>
-          <t>HER</t>
-        </is>
-      </c>
       <c r="ES2" t="inlineStr">
         <is>
           <t>VAL</t>
@@ -1842,19 +1812,27 @@
         </is>
       </c>
       <c r="EW2" t="n">
-        <v>40</v>
-      </c>
-      <c r="EX2" t="n">
-        <v>10</v>
-      </c>
-      <c r="EY2" t="n">
-        <v>10</v>
-      </c>
-      <c r="EZ2" t="n">
-        <v>10</v>
-      </c>
-      <c r="FA2" t="n">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="EX2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="EY2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="EZ2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="FA2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="FB2" t="inlineStr">
         <is>
@@ -1878,31 +1856,13 @@
       </c>
       <c r="FF2" t="inlineStr">
         <is>
-          <t>ALEJANDRO MO</t>
+          <t>JULEN S</t>
         </is>
       </c>
       <c r="FG2" t="inlineStr">
         <is>
           <t>#TrialVIC_2021</t>
         </is>
-      </c>
-      <c r="FH2" t="n">
-        <v>40</v>
-      </c>
-      <c r="FI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FM2" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reading and writing in same file
</commit_message>
<xml_diff>
--- a/TRIAL_VMIX.xlsx
+++ b/TRIAL_VMIX.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FM2"/>
+  <dimension ref="A1:FN2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,840 +439,845 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>TITOL_START</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>TITOL_MITJA</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>TITOL_FINAL</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>TITOL_2_FINAL</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>SECCIO</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>I_POSICIO_1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>I_POSICIO_2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>I_POSICIO_3</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>I_POSICIO_4</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>I_POSICIO_5</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>I_POSICIO_6</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>I_POSICIO_7</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>I_POSICIO_8</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>I_BANDERA_1</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>I_BANDERA_2</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>I_BANDERA_3</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>I_BANDERA_4</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>I_BANDERA_5</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>I_BANDERA_6</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>I_BANDERA_7</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>I_BANDERA_8</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>I_PAIS_1</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>I_PAIS_2</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>I_PAIS_3</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>I_PAIS_4</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>I_PAIS_5</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>I_PAIS_6</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>I_PAIS_7</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>I_PAIS_8</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>I_PLAYER_1</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>I_PLAYER_2</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>I_PLAYER_3</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>I_PLAYER_4</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>I_PLAYER_5</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>I_PLAYER_6</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>I_PLAYER_7</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>I_PLAYER_8</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>I_PUNTS_1</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>I_PUNTS_2</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>I_PUNTS_3</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>I_PUNTS_4</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>I_PUNTS_5</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>I_PUNTS_6</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>I_PUNTS_7</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>I_PUNTS_8</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>I_S1_1</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>I_S1_2</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>I_S1_3</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>I_S1_4</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>I_S1_5</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>I_S1_6</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>I_S1_7</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>I_S1_8</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>I_S2_1</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>I_S2_2</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>I_S2_3</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>I_S2_4</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>I_S2_5</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>I_S2_6</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>I_S2_7</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>I_S2_8</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>I_S3_1</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>I_S3_2</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>I_S3_3</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>I_S3_4</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>I_S3_5</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>I_S3_6</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>I_S3_7</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>I_S3_8</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>I_S4_1</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>I_S4_2</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>I_S4_3</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>I_S4_4</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>I_S4_5</t>
         </is>
       </c>
-      <c r="BX1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>I_S4_6</t>
         </is>
       </c>
-      <c r="BY1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>I_S4_7</t>
         </is>
       </c>
-      <c r="BZ1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>I_S4_8</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>I_S5_1</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>I_S5_2</t>
         </is>
       </c>
-      <c r="CC1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>I_S5_3</t>
         </is>
       </c>
-      <c r="CD1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>I_S5_4</t>
         </is>
       </c>
-      <c r="CE1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>I_S5_5</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>I_S5_6</t>
         </is>
       </c>
-      <c r="CG1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>I_S5_7</t>
         </is>
       </c>
-      <c r="CH1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>I_S5_8</t>
         </is>
       </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>F_POSICIO_1</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>F_POSICIO_2</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>F_POSICIO_3</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>F_POSICIO_4</t>
         </is>
       </c>
-      <c r="CM1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>F_POSICIO_5</t>
         </is>
       </c>
-      <c r="CN1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>F_POSICIO_6</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>F_BANDERA_1</t>
         </is>
       </c>
-      <c r="CP1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>F_BANDERA_2</t>
         </is>
       </c>
-      <c r="CQ1" s="1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>F_BANDERA_3</t>
         </is>
       </c>
-      <c r="CR1" s="1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>F_BANDERA_4</t>
         </is>
       </c>
-      <c r="CS1" s="1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>F_BANDERA_5</t>
         </is>
       </c>
-      <c r="CT1" s="1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>F_BANDERA_6</t>
         </is>
       </c>
-      <c r="CU1" s="1" t="inlineStr">
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>F_PAIS_1</t>
         </is>
       </c>
-      <c r="CV1" s="1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>F_PAIS_2</t>
         </is>
       </c>
-      <c r="CW1" s="1" t="inlineStr">
+      <c r="CX1" s="1" t="inlineStr">
         <is>
           <t>F_PAIS_3</t>
         </is>
       </c>
-      <c r="CX1" s="1" t="inlineStr">
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>F_PAIS_4</t>
         </is>
       </c>
-      <c r="CY1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>F_PAIS_5</t>
         </is>
       </c>
-      <c r="CZ1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>F_PAIS_6</t>
         </is>
       </c>
-      <c r="DA1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>F_PLAYER_1</t>
         </is>
       </c>
-      <c r="DB1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>F_PLAYER_2</t>
         </is>
       </c>
-      <c r="DC1" s="1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>F_PLAYER_3</t>
         </is>
       </c>
-      <c r="DD1" s="1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>F_PLAYER_4</t>
         </is>
       </c>
-      <c r="DE1" s="1" t="inlineStr">
+      <c r="DF1" s="1" t="inlineStr">
         <is>
           <t>F_PLAYER_5</t>
         </is>
       </c>
-      <c r="DF1" s="1" t="inlineStr">
+      <c r="DG1" s="1" t="inlineStr">
         <is>
           <t>F_PLAYER_6</t>
         </is>
       </c>
-      <c r="DG1" s="1" t="inlineStr">
+      <c r="DH1" s="1" t="inlineStr">
         <is>
           <t>F_PUNTS_1</t>
         </is>
       </c>
-      <c r="DH1" s="1" t="inlineStr">
+      <c r="DI1" s="1" t="inlineStr">
         <is>
           <t>F_PUNTS_2</t>
         </is>
       </c>
-      <c r="DI1" s="1" t="inlineStr">
+      <c r="DJ1" s="1" t="inlineStr">
         <is>
           <t>F_PUNTS_3</t>
         </is>
       </c>
-      <c r="DJ1" s="1" t="inlineStr">
+      <c r="DK1" s="1" t="inlineStr">
         <is>
           <t>F_PUNTS_4</t>
         </is>
       </c>
-      <c r="DK1" s="1" t="inlineStr">
+      <c r="DL1" s="1" t="inlineStr">
         <is>
           <t>F_PUNTS_5</t>
         </is>
       </c>
-      <c r="DL1" s="1" t="inlineStr">
+      <c r="DM1" s="1" t="inlineStr">
         <is>
           <t>F_PUNTS_6</t>
         </is>
       </c>
-      <c r="DM1" s="1" t="inlineStr">
+      <c r="DN1" s="1" t="inlineStr">
         <is>
           <t>F_S1_1</t>
         </is>
       </c>
-      <c r="DN1" s="1" t="inlineStr">
+      <c r="DO1" s="1" t="inlineStr">
         <is>
           <t>F_S1_2</t>
         </is>
       </c>
-      <c r="DO1" s="1" t="inlineStr">
+      <c r="DP1" s="1" t="inlineStr">
         <is>
           <t>F_S1_3</t>
         </is>
       </c>
-      <c r="DP1" s="1" t="inlineStr">
+      <c r="DQ1" s="1" t="inlineStr">
         <is>
           <t>F_S1_4</t>
         </is>
       </c>
-      <c r="DQ1" s="1" t="inlineStr">
+      <c r="DR1" s="1" t="inlineStr">
         <is>
           <t>F_S1_5</t>
         </is>
       </c>
-      <c r="DR1" s="1" t="inlineStr">
+      <c r="DS1" s="1" t="inlineStr">
         <is>
           <t>F_S1_6</t>
         </is>
       </c>
-      <c r="DS1" s="1" t="inlineStr">
+      <c r="DT1" s="1" t="inlineStr">
         <is>
           <t>F_S2_1</t>
         </is>
       </c>
-      <c r="DT1" s="1" t="inlineStr">
+      <c r="DU1" s="1" t="inlineStr">
         <is>
           <t>F_S2_2</t>
         </is>
       </c>
-      <c r="DU1" s="1" t="inlineStr">
+      <c r="DV1" s="1" t="inlineStr">
         <is>
           <t>F_S2_3</t>
         </is>
       </c>
-      <c r="DV1" s="1" t="inlineStr">
+      <c r="DW1" s="1" t="inlineStr">
         <is>
           <t>F_S2_4</t>
         </is>
       </c>
-      <c r="DW1" s="1" t="inlineStr">
+      <c r="DX1" s="1" t="inlineStr">
         <is>
           <t>F_S2_5</t>
         </is>
       </c>
-      <c r="DX1" s="1" t="inlineStr">
+      <c r="DY1" s="1" t="inlineStr">
         <is>
           <t>F_S2_6</t>
         </is>
       </c>
-      <c r="DY1" s="1" t="inlineStr">
+      <c r="DZ1" s="1" t="inlineStr">
         <is>
           <t>F_S3_1</t>
         </is>
       </c>
-      <c r="DZ1" s="1" t="inlineStr">
+      <c r="EA1" s="1" t="inlineStr">
         <is>
           <t>F_S3_2</t>
         </is>
       </c>
-      <c r="EA1" s="1" t="inlineStr">
+      <c r="EB1" s="1" t="inlineStr">
         <is>
           <t>F_S3_3</t>
         </is>
       </c>
-      <c r="EB1" s="1" t="inlineStr">
+      <c r="EC1" s="1" t="inlineStr">
         <is>
           <t>F_S3_4</t>
         </is>
       </c>
-      <c r="EC1" s="1" t="inlineStr">
+      <c r="ED1" s="1" t="inlineStr">
         <is>
           <t>F_S3_5</t>
         </is>
       </c>
-      <c r="ED1" s="1" t="inlineStr">
+      <c r="EE1" s="1" t="inlineStr">
         <is>
           <t>F_S3_6</t>
         </is>
       </c>
-      <c r="EE1" s="1" t="inlineStr">
+      <c r="EF1" s="1" t="inlineStr">
         <is>
           <t>F_S4_1</t>
         </is>
       </c>
-      <c r="EF1" s="1" t="inlineStr">
+      <c r="EG1" s="1" t="inlineStr">
         <is>
           <t>F_S4_2</t>
         </is>
       </c>
-      <c r="EG1" s="1" t="inlineStr">
+      <c r="EH1" s="1" t="inlineStr">
         <is>
           <t>F_S4_3</t>
         </is>
       </c>
-      <c r="EH1" s="1" t="inlineStr">
+      <c r="EI1" s="1" t="inlineStr">
         <is>
           <t>F_S4_4</t>
         </is>
       </c>
-      <c r="EI1" s="1" t="inlineStr">
+      <c r="EJ1" s="1" t="inlineStr">
         <is>
           <t>F_S4_5</t>
         </is>
       </c>
-      <c r="EJ1" s="1" t="inlineStr">
+      <c r="EK1" s="1" t="inlineStr">
         <is>
           <t>F_S4_6</t>
         </is>
       </c>
-      <c r="EK1" s="1" t="inlineStr">
+      <c r="EL1" s="1" t="inlineStr">
         <is>
           <t>F_S5_1</t>
         </is>
       </c>
-      <c r="EL1" s="1" t="inlineStr">
+      <c r="EM1" s="1" t="inlineStr">
         <is>
           <t>F_S5_2</t>
         </is>
       </c>
-      <c r="EM1" s="1" t="inlineStr">
+      <c r="EN1" s="1" t="inlineStr">
         <is>
           <t>F_S5_3</t>
         </is>
       </c>
-      <c r="EN1" s="1" t="inlineStr">
+      <c r="EO1" s="1" t="inlineStr">
         <is>
           <t>F_S5_4</t>
         </is>
       </c>
-      <c r="EO1" s="1" t="inlineStr">
+      <c r="EP1" s="1" t="inlineStr">
         <is>
           <t>F_S5_5</t>
         </is>
       </c>
-      <c r="EP1" s="1" t="inlineStr">
+      <c r="EQ1" s="1" t="inlineStr">
         <is>
           <t>F_S5_6</t>
         </is>
       </c>
-      <c r="EQ1" s="1" t="inlineStr">
+      <c r="ER1" s="1" t="inlineStr">
         <is>
           <t>F_ABR_1</t>
         </is>
       </c>
-      <c r="ER1" s="1" t="inlineStr">
+      <c r="ES1" s="1" t="inlineStr">
         <is>
           <t>F_ABR_2</t>
         </is>
       </c>
-      <c r="ES1" s="1" t="inlineStr">
+      <c r="ET1" s="1" t="inlineStr">
         <is>
           <t>F_ABR_3</t>
         </is>
       </c>
-      <c r="ET1" s="1" t="inlineStr">
+      <c r="EU1" s="1" t="inlineStr">
         <is>
           <t>F_ABR_4</t>
         </is>
       </c>
-      <c r="EU1" s="1" t="inlineStr">
+      <c r="EV1" s="1" t="inlineStr">
         <is>
           <t>F_ABR_5</t>
         </is>
       </c>
-      <c r="EV1" s="1" t="inlineStr">
+      <c r="EW1" s="1" t="inlineStr">
         <is>
           <t>F_ABR_6</t>
         </is>
       </c>
-      <c r="EW1" s="1" t="inlineStr">
+      <c r="EX1" s="1" t="inlineStr">
         <is>
           <t>C_PUNTS_SECCIO</t>
         </is>
       </c>
-      <c r="EX1" s="1" t="inlineStr">
+      <c r="EY1" s="1" t="inlineStr">
         <is>
           <t>C_PUNTS_P1</t>
         </is>
       </c>
-      <c r="EY1" s="1" t="inlineStr">
+      <c r="EZ1" s="1" t="inlineStr">
         <is>
           <t>C_PUNTS_P2</t>
         </is>
       </c>
-      <c r="EZ1" s="1" t="inlineStr">
+      <c r="FA1" s="1" t="inlineStr">
         <is>
           <t>C_PUNTS_P3</t>
         </is>
       </c>
-      <c r="FA1" s="1" t="inlineStr">
+      <c r="FB1" s="1" t="inlineStr">
         <is>
           <t>C_PUNTS_P4</t>
         </is>
       </c>
-      <c r="FB1" s="1" t="inlineStr">
+      <c r="FC1" s="1" t="inlineStr">
         <is>
           <t>C_PUNTS_P5</t>
         </is>
       </c>
-      <c r="FC1" s="1" t="inlineStr">
+      <c r="FD1" s="1" t="inlineStr">
         <is>
           <t>C_PUNTS_P6</t>
         </is>
       </c>
-      <c r="FD1" s="1" t="inlineStr">
+      <c r="FE1" s="1" t="inlineStr">
         <is>
           <t>C_BANDERA</t>
         </is>
       </c>
-      <c r="FE1" s="1" t="inlineStr">
+      <c r="FF1" s="1" t="inlineStr">
         <is>
           <t>C_PAIS</t>
         </is>
       </c>
-      <c r="FF1" s="1" t="inlineStr">
+      <c r="FG1" s="1" t="inlineStr">
         <is>
           <t>C_PLAYER</t>
         </is>
       </c>
-      <c r="FG1" s="1" t="inlineStr">
+      <c r="FH1" s="1" t="inlineStr">
         <is>
           <t>hashtag</t>
         </is>
       </c>
-      <c r="FH1" s="1" t="inlineStr">
+      <c r="FI1" s="1" t="inlineStr">
         <is>
           <t>1_PUNTS_SECCIO</t>
         </is>
       </c>
-      <c r="FI1" s="1" t="inlineStr">
+      <c r="FJ1" s="1" t="inlineStr">
         <is>
           <t>2_PUNTS_SECCIO</t>
         </is>
       </c>
-      <c r="FJ1" s="1" t="inlineStr">
+      <c r="FK1" s="1" t="inlineStr">
         <is>
           <t>3_PUNTS_SECCIO</t>
         </is>
       </c>
-      <c r="FK1" s="1" t="inlineStr">
+      <c r="FL1" s="1" t="inlineStr">
         <is>
           <t>4_PUNTS_SECCIO</t>
         </is>
       </c>
-      <c r="FL1" s="1" t="inlineStr">
+      <c r="FM1" s="1" t="inlineStr">
         <is>
           <t>5_PUNTS_SECCIO</t>
         </is>
       </c>
-      <c r="FM1" s="1" t="inlineStr">
+      <c r="FN1" s="1" t="inlineStr">
         <is>
           <t>6_PUNTS_SECCIO</t>
         </is>
@@ -1282,201 +1287,201 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>TRIALS - MEN ELITE 26" - FINALS - START LIST</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>TRIALS - MEN ELITE 26" - FINALS - AFTER SECTION 1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve">TRIALS - MEN ELITE 26" - FINALS - RESULTS </t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>MEN ELITE - FINAL</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>SECTION 1</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>SECTION 2</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>7</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>5</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>6</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>4</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>9</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>17</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>28</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\ger.png</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>GER</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
         <is>
           <t>VINCENT H</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>ALEJANDRO MO</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>NICOLAS V</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>BORJA CO</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>ELOI PA</t>
         </is>
       </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>JULEN S</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>LOUIS GRILLON</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>DOMINIK OSWALD</t>
         </is>
       </c>
-      <c r="AM2" t="n">
+      <c r="AN2" t="n">
         <v>540</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AO2" t="n">
         <v>530</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>520</v>
       </c>
       <c r="AP2" t="n">
         <v>520</v>
       </c>
       <c r="AQ2" t="n">
+        <v>520</v>
+      </c>
+      <c r="AR2" t="n">
         <v>490</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AS2" t="n">
         <v>480</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AT2" t="n">
         <v>470</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="AU2" t="n">
         <v>460</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>120</v>
       </c>
       <c r="AV2" t="n">
         <v>120</v>
@@ -1485,13 +1490,13 @@
         <v>120</v>
       </c>
       <c r="AX2" t="n">
+        <v>120</v>
+      </c>
+      <c r="AY2" t="n">
         <v>100</v>
       </c>
-      <c r="AY2" t="n">
+      <c r="AZ2" t="n">
         <v>90</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>120</v>
       </c>
       <c r="BA2" t="n">
         <v>120</v>
@@ -1500,10 +1505,10 @@
         <v>120</v>
       </c>
       <c r="BC2" t="n">
+        <v>120</v>
+      </c>
+      <c r="BD2" t="n">
         <v>110</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>120</v>
       </c>
       <c r="BE2" t="n">
         <v>120</v>
@@ -1515,79 +1520,79 @@
         <v>120</v>
       </c>
       <c r="BH2" t="n">
+        <v>120</v>
+      </c>
+      <c r="BI2" t="n">
         <v>110</v>
       </c>
-      <c r="BI2" t="n">
+      <c r="BJ2" t="n">
         <v>90</v>
       </c>
-      <c r="BJ2" t="n">
+      <c r="BK2" t="n">
         <v>100</v>
       </c>
-      <c r="BK2" t="n">
+      <c r="BL2" t="n">
         <v>120</v>
       </c>
-      <c r="BL2" t="n">
+      <c r="BM2" t="n">
         <v>60</v>
       </c>
-      <c r="BM2" t="n">
+      <c r="BN2" t="n">
         <v>110</v>
       </c>
-      <c r="BN2" t="n">
+      <c r="BO2" t="n">
         <v>90</v>
       </c>
-      <c r="BO2" t="n">
+      <c r="BP2" t="n">
         <v>120</v>
       </c>
-      <c r="BP2" t="n">
+      <c r="BQ2" t="n">
         <v>110</v>
       </c>
-      <c r="BQ2" t="n">
+      <c r="BR2" t="n">
         <v>120</v>
       </c>
-      <c r="BR2" t="n">
+      <c r="BS2" t="n">
         <v>90</v>
       </c>
-      <c r="BS2" t="n">
+      <c r="BT2" t="n">
         <v>110</v>
       </c>
-      <c r="BT2" t="n">
+      <c r="BU2" t="n">
         <v>120</v>
       </c>
-      <c r="BU2" t="n">
+      <c r="BV2" t="n">
         <v>110</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>120</v>
       </c>
       <c r="BW2" t="n">
         <v>120</v>
       </c>
       <c r="BX2" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="BY2" t="n">
         <v>110</v>
       </c>
       <c r="BZ2" t="n">
+        <v>110</v>
+      </c>
+      <c r="CA2" t="n">
         <v>120</v>
       </c>
-      <c r="CA2" t="n">
+      <c r="CB2" t="n">
         <v>80</v>
       </c>
-      <c r="CB2" t="n">
+      <c r="CC2" t="n">
         <v>110</v>
       </c>
-      <c r="CC2" t="n">
+      <c r="CD2" t="n">
         <v>60</v>
       </c>
-      <c r="CD2" t="n">
+      <c r="CE2" t="n">
         <v>90</v>
       </c>
-      <c r="CE2" t="n">
+      <c r="CF2" t="n">
         <v>40</v>
-      </c>
-      <c r="CF2" t="n">
-        <v>30</v>
       </c>
       <c r="CG2" t="n">
         <v>30</v>
@@ -1596,310 +1601,306 @@
         <v>30</v>
       </c>
       <c r="CI2" t="n">
+        <v>30</v>
+      </c>
+      <c r="CJ2" t="n">
         <v>1</v>
       </c>
-      <c r="CJ2" t="n">
+      <c r="CK2" t="n">
         <v>2</v>
       </c>
-      <c r="CK2" t="n">
+      <c r="CL2" t="n">
         <v>3</v>
       </c>
-      <c r="CL2" t="n">
+      <c r="CM2" t="n">
         <v>4</v>
       </c>
-      <c r="CM2" t="n">
+      <c r="CN2" t="n">
         <v>5</v>
       </c>
-      <c r="CN2" t="n">
+      <c r="CO2" t="n">
         <v>6</v>
       </c>
-      <c r="CO2" t="inlineStr">
+      <c r="CP2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
         </is>
       </c>
-      <c r="CP2" t="inlineStr">
+      <c r="CQ2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="CQ2" t="inlineStr">
+      <c r="CR2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
         </is>
       </c>
-      <c r="CR2" t="inlineStr">
+      <c r="CS2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="CS2" t="inlineStr">
+      <c r="CT2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="CT2" t="inlineStr">
+      <c r="CU2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="CU2" t="inlineStr">
+      <c r="CV2" t="inlineStr">
         <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="CV2" t="inlineStr">
+      <c r="CW2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="CW2" t="inlineStr">
+      <c r="CX2" t="inlineStr">
         <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="CX2" t="inlineStr">
+      <c r="CY2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="CY2" t="inlineStr">
+      <c r="CZ2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="CZ2" t="inlineStr">
+      <c r="DA2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="DA2" t="inlineStr">
+      <c r="DB2" t="inlineStr">
+        <is>
+          <t>NICOLAS V</t>
+        </is>
+      </c>
+      <c r="DC2" t="inlineStr">
+        <is>
+          <t>BORJA CO</t>
+        </is>
+      </c>
+      <c r="DD2" t="inlineStr">
         <is>
           <t>VINCENT H</t>
         </is>
       </c>
-      <c r="DB2" t="inlineStr">
+      <c r="DE2" t="inlineStr">
         <is>
           <t>ALEJANDRO MO</t>
         </is>
       </c>
-      <c r="DC2" t="inlineStr">
-        <is>
-          <t>NICOLAS V</t>
-        </is>
-      </c>
-      <c r="DD2" t="inlineStr">
+      <c r="DF2" t="inlineStr">
+        <is>
+          <t>ELOI PA</t>
+        </is>
+      </c>
+      <c r="DG2" t="inlineStr">
+        <is>
+          <t>JULEN S</t>
+        </is>
+      </c>
+      <c r="DH2" t="n">
+        <v>40</v>
+      </c>
+      <c r="DI2" t="n">
+        <v>30</v>
+      </c>
+      <c r="DJ2" t="n">
+        <v>20</v>
+      </c>
+      <c r="DK2" t="n">
+        <v>20</v>
+      </c>
+      <c r="DL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP2" t="n">
+        <v>20</v>
+      </c>
+      <c r="DQ2" t="n">
+        <v>20</v>
+      </c>
+      <c r="DR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT2" t="n">
+        <v>40</v>
+      </c>
+      <c r="DU2" t="n">
+        <v>30</v>
+      </c>
+      <c r="DV2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DY2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="ER2" t="inlineStr">
+        <is>
+          <t>VAL</t>
+        </is>
+      </c>
+      <c r="ES2" t="inlineStr">
+        <is>
+          <t>CON</t>
+        </is>
+      </c>
+      <c r="ET2" t="inlineStr">
+        <is>
+          <t>HER</t>
+        </is>
+      </c>
+      <c r="EU2" t="inlineStr">
+        <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="EV2" t="inlineStr">
+        <is>
+          <t>PAL</t>
+        </is>
+      </c>
+      <c r="EW2" t="inlineStr">
+        <is>
+          <t>SAE</t>
+        </is>
+      </c>
+      <c r="EX2" t="n">
+        <v>30</v>
+      </c>
+      <c r="EY2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="EZ2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="FA2" t="n">
+        <v>10</v>
+      </c>
+      <c r="FB2" t="n">
+        <v>10</v>
+      </c>
+      <c r="FC2" t="n">
+        <v>10</v>
+      </c>
+      <c r="FD2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="FE2" t="inlineStr">
+        <is>
+          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
+        </is>
+      </c>
+      <c r="FF2" t="inlineStr">
+        <is>
+          <t>ESP</t>
+        </is>
+      </c>
+      <c r="FG2" t="inlineStr">
         <is>
           <t>BORJA CO</t>
         </is>
       </c>
-      <c r="DE2" t="inlineStr">
-        <is>
-          <t>ELOI PA</t>
-        </is>
-      </c>
-      <c r="DF2" t="inlineStr">
-        <is>
-          <t>JULEN S</t>
-        </is>
-      </c>
-      <c r="DG2" t="n">
-        <v>10</v>
-      </c>
-      <c r="DH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DM2" t="n">
-        <v>10</v>
-      </c>
-      <c r="DN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DQ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DR2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DS2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DT2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DU2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DV2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DW2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DX2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DY2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DZ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="ED2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EG2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EQ2" t="inlineStr">
-        <is>
-          <t>HER</t>
-        </is>
-      </c>
-      <c r="ER2" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
-      <c r="ES2" t="inlineStr">
-        <is>
-          <t>VAL</t>
-        </is>
-      </c>
-      <c r="ET2" t="inlineStr">
-        <is>
-          <t>CON</t>
-        </is>
-      </c>
-      <c r="EU2" t="inlineStr">
-        <is>
-          <t>PAL</t>
-        </is>
-      </c>
-      <c r="EV2" t="inlineStr">
-        <is>
-          <t>SAE</t>
-        </is>
-      </c>
-      <c r="EW2" t="n">
-        <v>10</v>
-      </c>
-      <c r="EX2" t="n">
-        <v>10</v>
-      </c>
-      <c r="EY2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="EZ2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="FA2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="FB2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="FC2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="FD2" t="inlineStr">
-        <is>
-          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
-        </is>
-      </c>
-      <c r="FE2" t="inlineStr">
-        <is>
-          <t>FRA</t>
-        </is>
-      </c>
-      <c r="FF2" t="inlineStr">
-        <is>
-          <t>VINCENT H</t>
-        </is>
-      </c>
-      <c r="FG2" t="inlineStr">
+      <c r="FH2" t="inlineStr">
         <is>
           <t>#TrialVIC_2021</t>
         </is>
       </c>
-      <c r="FH2" t="n">
-        <v>10</v>
-      </c>
       <c r="FI2" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="FJ2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="FK2" t="n">
         <v>0</v>
@@ -1908,6 +1909,9 @@
         <v>0</v>
       </c>
       <c r="FM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="FN2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update yellow keys when player change
</commit_message>
<xml_diff>
--- a/TRIAL_VMIX.xlsx
+++ b/TRIAL_VMIX.xlsx
@@ -1729,74 +1729,74 @@
       </c>
       <c r="CZ2" t="inlineStr">
         <is>
+          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
+        </is>
+      </c>
+      <c r="DA2" t="inlineStr">
+        <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
         </is>
       </c>
-      <c r="DA2" t="inlineStr">
+      <c r="DB2" t="inlineStr">
+        <is>
+          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
+        </is>
+      </c>
+      <c r="DC2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="DB2" t="inlineStr">
-        <is>
-          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\fra.png</t>
-        </is>
-      </c>
-      <c r="DC2" t="inlineStr">
+      <c r="DD2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="DD2" t="inlineStr">
+      <c r="DE2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
-      <c r="DE2" t="inlineStr">
-        <is>
-          <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
-        </is>
-      </c>
       <c r="DF2" t="inlineStr">
         <is>
+          <t>ESP</t>
+        </is>
+      </c>
+      <c r="DG2" t="inlineStr">
+        <is>
           <t>FRA</t>
         </is>
       </c>
-      <c r="DG2" t="inlineStr">
+      <c r="DH2" t="inlineStr">
+        <is>
+          <t>FRA</t>
+        </is>
+      </c>
+      <c r="DI2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="DH2" t="inlineStr">
-        <is>
-          <t>FRA</t>
-        </is>
-      </c>
-      <c r="DI2" t="inlineStr">
+      <c r="DJ2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="DJ2" t="inlineStr">
+      <c r="DK2" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="DK2" t="inlineStr">
-        <is>
-          <t>ESP</t>
-        </is>
-      </c>
       <c r="DL2" t="inlineStr">
         <is>
+          <t>ALEJANDRO MO</t>
+        </is>
+      </c>
+      <c r="DM2" t="inlineStr">
+        <is>
           <t>VINCENT H</t>
         </is>
       </c>
-      <c r="DM2" t="inlineStr">
-        <is>
-          <t>ALEJANDRO MO</t>
-        </is>
-      </c>
       <c r="DN2" t="inlineStr">
         <is>
           <t>NICOLAS V</t>
@@ -1818,10 +1818,10 @@
         </is>
       </c>
       <c r="DR2" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="DS2" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="DT2" t="n">
         <v>0</v>
@@ -1839,61 +1839,61 @@
         <v>30</v>
       </c>
       <c r="DY2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EP2" t="n">
         <v>30</v>
       </c>
-      <c r="DZ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="ED2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EG2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP2" t="n">
-        <v>0</v>
-      </c>
       <c r="EQ2" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="ER2" t="n">
         <v>0</v>
@@ -1927,14 +1927,14 @@
       </c>
       <c r="FB2" t="inlineStr">
         <is>
+          <t>MON</t>
+        </is>
+      </c>
+      <c r="FC2" t="inlineStr">
+        <is>
           <t>HER</t>
         </is>
       </c>
-      <c r="FC2" t="inlineStr">
-        <is>
-          <t>MON</t>
-        </is>
-      </c>
       <c r="FD2" t="inlineStr">
         <is>
           <t>VAL</t>
@@ -1957,52 +1957,46 @@
       </c>
       <c r="FH2" t="inlineStr">
         <is>
-          <t>SECTION 3</t>
+          <t>SECTION 1</t>
         </is>
       </c>
       <c r="FI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FJ2" t="inlineStr">
+        <v>30</v>
+      </c>
+      <c r="FJ2" t="n">
+        <v>10</v>
+      </c>
+      <c r="FK2" t="n">
+        <v>10</v>
+      </c>
+      <c r="FL2" t="n">
+        <v>10</v>
+      </c>
+      <c r="FM2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="FK2" t="inlineStr">
+      <c r="FN2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="FL2" t="inlineStr">
+      <c r="FO2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="FM2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="FN2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="FO2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="FP2" t="inlineStr">
         <is>
           <t>C:\TRIAL_2021\VMIX\MATERIAL\BANDERES\esp.png</t>
         </is>
       </c>
       <c r="FQ2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="FR2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="FS2" t="inlineStr">
         <is>
@@ -2011,7 +2005,7 @@
       </c>
       <c r="FT2" t="inlineStr">
         <is>
-          <t>BORJA CO</t>
+          <t>ALEJANDRO MO</t>
         </is>
       </c>
       <c r="FU2" t="inlineStr">
@@ -2021,14 +2015,14 @@
       </c>
       <c r="FV2" t="inlineStr">
         <is>
-          <t>SECTION 1</t>
+          <t>SECTION 4</t>
         </is>
       </c>
       <c r="FW2" t="n">
         <v>30</v>
       </c>
       <c r="FX2" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="FY2" t="n">
         <v>0</v>
@@ -3244,7 +3238,7 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -3253,13 +3247,13 @@
         <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N18" t="n">
         <v>0</v>
@@ -3271,10 +3265,10 @@
         <v>0</v>
       </c>
       <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
         <v>1</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -3283,7 +3277,7 @@
         <v>4</v>
       </c>
       <c r="U18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
@@ -3329,13 +3323,13 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L19" t="n">
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
@@ -3347,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" t="n">
         <v>0</v>
@@ -3356,10 +3350,10 @@
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>

</xml_diff>